<commit_message>
time calculation alg Fix
</commit_message>
<xml_diff>
--- a/test/times.xlsx
+++ b/test/times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notsi\Documents\git\Progetto_ASD_py\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F3FFEBA-053B-48F8-89A8-684CB288BC3C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{08075C12-08E0-4337-B356-1BE8759CAC1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25680" yWindow="3120" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
@@ -30,7 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>mergesort</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -81,6 +85,957 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Foglio1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.6898749981607699E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1379407405853198E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6765526958874199E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.7631555578925394E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.55242729187011E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.101595252990722</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.14046108064980301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16186569255331201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.191987714442339</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.21576313525438301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25560941199461601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F6A3-498A-A7DE-8B4CB086EA77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="356527760"/>
+        <c:axId val="350935200"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="356527760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="350935200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="350935200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="356527760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E73FD58-1852-4B01-9AB6-76EE363C655A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,112 +1348,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1000</v>
-      </c>
-      <c r="B1">
-        <v>1.6898749981607699E-2</v>
+      <c r="B1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="B2">
-        <v>4.1379407405853198E-2</v>
+        <v>1.6898749981607699E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3000</v>
+        <v>2000</v>
+      </c>
+      <c r="B3">
+        <v>4.1379407405853198E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4000</v>
+        <v>3000</v>
+      </c>
+      <c r="B4">
+        <v>5.6765526958874199E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5000</v>
+        <v>4000</v>
+      </c>
+      <c r="B5">
+        <v>8.7631555578925394E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6000</v>
+        <v>5000</v>
+      </c>
+      <c r="B6">
+        <v>8.55242729187011E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7000</v>
+        <v>6000</v>
+      </c>
+      <c r="B7">
+        <v>0.101595252990722</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8000</v>
+        <v>7000</v>
+      </c>
+      <c r="B8">
+        <v>0.14046108064980301</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9000</v>
+        <v>8000</v>
+      </c>
+      <c r="B9">
+        <v>0.16186569255331201</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10000</v>
+        <v>9000</v>
+      </c>
+      <c r="B10">
+        <v>0.191987714442339</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11000</v>
+        <v>10000</v>
+      </c>
+      <c r="B11">
+        <v>0.21576313525438301</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12000</v>
+        <v>11000</v>
+      </c>
+      <c r="B12">
+        <v>0.25560941199461601</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14000</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>15000</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>16000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>17000</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>18000</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>19000</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
debug lwm alg fix
</commit_message>
<xml_diff>
--- a/test/times.xlsx
+++ b/test/times.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notsi\Documents\git\Progetto_ASD_py\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{08075C12-08E0-4337-B356-1BE8759CAC1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCFAB75-4D9C-40DC-B20D-9A8D82DD9ADA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25680" yWindow="3120" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-27105" yWindow="1155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -30,15 +30,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>mergesort</t>
+    <t>nlogn</t>
+  </si>
+  <si>
+    <t>n2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -102,6 +106,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Andamento Tempi</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -152,75 +181,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Foglio1!$A$2:$A$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$B$2:$B$21</c:f>
@@ -228,37 +188,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.6898749981607699E-2</c:v>
+                  <c:v>4.9649100303649904E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1379407405853198E-2</c:v>
+                  <c:v>9.6226436751229404E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.6765526958874199E-2</c:v>
+                  <c:v>1.42114275693893E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.7631555578925394E-2</c:v>
+                  <c:v>1.9984919428825298E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.55242729187011E-2</c:v>
+                  <c:v>2.5279560414227499E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.101595252990722</c:v>
+                  <c:v>2.97260006268819E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14046108064980301</c:v>
+                  <c:v>3.3352933431926503E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16186569255331201</c:v>
+                  <c:v>4.1764576184122097E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.191987714442339</c:v>
+                  <c:v>4.3446660669226297E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.21576313525438301</c:v>
+                  <c:v>4.7313038706779401E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.25560941199461601</c:v>
+                  <c:v>5.1609424087736298E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5210474917763097E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.2611039280891401E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.4773599969016105E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8748948971430399E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.69133097595638E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.3617520332336395E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.9669313695695599E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.2817313803566795E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -267,6 +251,49 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F6A3-498A-A7DE-8B4CB086EA77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.4304305930057999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7364985868796999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9573364306842504E-4</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>1.23982408383917E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E36C-4B51-B548-F2A9E34C6CCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1001,16 +1028,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1334,153 +1361,196 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
       <c r="B2">
-        <v>1.6898749981607699E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.9649100303649904E-3</v>
+      </c>
+      <c r="C2">
+        <v>2.4304305930057999E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
       <c r="B3">
-        <v>4.1379407405853198E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9.6226436751229404E-3</v>
+      </c>
+      <c r="C3">
+        <v>4.7364985868796999E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3000</v>
       </c>
       <c r="B4">
-        <v>5.6765526958874199E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.42114275693893E-2</v>
+      </c>
+      <c r="C4">
+        <v>6.9573364306842504E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4000</v>
       </c>
       <c r="B5">
-        <v>8.7631555578925394E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.9984919428825298E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.23982408383917E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5000</v>
       </c>
       <c r="B6">
-        <v>8.55242729187011E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.5279560414227499E-2</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6000</v>
       </c>
       <c r="B7">
-        <v>0.101595252990722</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.97260006268819E-2</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7000</v>
       </c>
       <c r="B8">
-        <v>0.14046108064980301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.3352933431926503E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8000</v>
       </c>
       <c r="B9">
-        <v>0.16186569255331201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.1764576184122097E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9000</v>
       </c>
       <c r="B10">
-        <v>0.191987714442339</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.3446660669226297E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10000</v>
       </c>
       <c r="B11">
-        <v>0.21576313525438301</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.7313038706779401E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11000</v>
       </c>
       <c r="B12">
-        <v>0.25560941199461601</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.1609424087736298E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12000</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>5.5210474917763097E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13000</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>6.2611039280891401E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14000</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>6.4773599969016105E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15000</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>6.8748948971430399E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16000</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>7.69133097595638E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17000</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>8.3617520332336395E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18000</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>8.9669313695695599E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19000</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>9.2817313803566795E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20000</v>
       </c>

</xml_diff>